<commit_message>
Cambios en el nombre bd, cambio en bd y conexion de vistas director administrador
</commit_message>
<xml_diff>
--- a/archivos/copia_estudiantes.xlsx
+++ b/archivos/copia_estudiantes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="INFO ESTUDIANTE" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t xml:space="preserve">CODIGO</t>
   </si>
@@ -106,6 +106,24 @@
   </si>
   <si>
     <t xml:space="preserve">FGSIANS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aven 7 con 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17@ufps.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False</t>
   </si>
   <si>
     <t xml:space="preserve">LECTUR</t>
@@ -130,9 +148,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -213,7 +232,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -230,11 +249,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -259,10 +282,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S3" activeCellId="0" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -272,7 +295,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.62"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="11" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.37"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.51"/>
@@ -373,7 +396,7 @@
         <v>9</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>42005</v>
+        <v>43831</v>
       </c>
       <c r="M2" s="4" t="n">
         <v>38809</v>
@@ -395,12 +418,73 @@
       </c>
       <c r="S2" s="5" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1111111</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>777777</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>171717171</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>717171</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L3" s="6" t="n">
+        <v>36651</v>
+      </c>
+      <c r="M3" s="6" t="n">
+        <v>36651</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>1111111</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>1212</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>1313</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="ivan@gmail.com"/>
     <hyperlink ref="J2" r:id="rId2" display="ivan@ufps.edu.co"/>
+    <hyperlink ref="F3" r:id="rId3" display="17@gmail.com"/>
+    <hyperlink ref="J3" r:id="rId4" display="17@ufps.edu.co"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -420,7 +504,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -430,22 +514,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,8 +552,28 @@
         <v>27</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>61</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>61</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>61</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>61</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>1313</v>
+      </c>
+    </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="6"/>
+      <c r="F8" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -487,10 +591,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -500,22 +604,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -534,10 +638,30 @@
       <c r="E2" s="5" t="n">
         <v>70</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>26</v>
+      <c r="F2" s="5" t="n">
+        <v>1212</v>
       </c>
       <c r="G2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>1212</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
retoques en las vistas egresado, administrativo y login
</commit_message>
<xml_diff>
--- a/archivos/copia_estudiantes.xlsx
+++ b/archivos/copia_estudiantes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="INFO ESTUDIANTE" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t xml:space="preserve">CODIGO</t>
   </si>
@@ -106,6 +106,24 @@
   </si>
   <si>
     <t xml:space="preserve">FGSIANS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aven 7 con 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17@ufps.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False</t>
   </si>
   <si>
     <t xml:space="preserve">LECTUR</t>
@@ -130,9 +148,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -213,7 +232,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -230,11 +249,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -259,10 +282,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S3" activeCellId="0" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -272,7 +295,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.62"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="11" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.37"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.51"/>
@@ -373,7 +396,7 @@
         <v>9</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>42005</v>
+        <v>43831</v>
       </c>
       <c r="M2" s="4" t="n">
         <v>38809</v>
@@ -395,12 +418,73 @@
       </c>
       <c r="S2" s="5" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1111111</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>777777</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>171717171</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>717171</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L3" s="6" t="n">
+        <v>36651</v>
+      </c>
+      <c r="M3" s="6" t="n">
+        <v>36651</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>1111111</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>1212</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>1313</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="ivan@gmail.com"/>
     <hyperlink ref="J2" r:id="rId2" display="ivan@ufps.edu.co"/>
+    <hyperlink ref="F3" r:id="rId3" display="17@gmail.com"/>
+    <hyperlink ref="J3" r:id="rId4" display="17@ufps.edu.co"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -420,7 +504,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -430,22 +514,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,8 +552,28 @@
         <v>27</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>61</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>61</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>61</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>61</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>1313</v>
+      </c>
+    </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="6"/>
+      <c r="F8" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -487,10 +591,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -500,22 +604,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -534,10 +638,30 @@
       <c r="E2" s="5" t="n">
         <v>70</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>26</v>
+      <c r="F2" s="5" t="n">
+        <v>1212</v>
       </c>
       <c r="G2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>1212</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Correcion de promedio, y materias aprobadas
</commit_message>
<xml_diff>
--- a/archivos/copia_estudiantes.xlsx
+++ b/archivos/copia_estudiantes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t xml:space="preserve">CODIGO</t>
   </si>
@@ -142,6 +142,21 @@
   </si>
   <si>
     <t xml:space="preserve">Hola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12@ufps.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13@ufps.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14@ufps.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15@ufps.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16@ufps.edu.co</t>
   </si>
   <si>
     <t xml:space="preserve">LECTURA</t>
@@ -287,7 +302,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -332,16 +347,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -429,10 +440,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T4" activeCellId="1" sqref="A1:F4 T4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -440,7 +451,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.91"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.24"/>
@@ -448,11 +459,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="29.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="21.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="21.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="24.62"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="11.52"/>
   </cols>
@@ -517,7 +528,7 @@
       </c>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>1151612</v>
       </c>
@@ -576,7 +587,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>1111111</v>
       </c>
@@ -635,7 +646,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>555555</v>
       </c>
@@ -654,19 +665,19 @@
       <c r="F4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="4" t="n">
         <v>23421</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="4" t="n">
         <v>9</v>
       </c>
       <c r="L4" s="9" t="n">
@@ -678,83 +689,706 @@
       <c r="N4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="O4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="0" t="n">
+      <c r="P4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="Q4" s="0" t="n">
+      <c r="Q4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="R4" s="0" t="n">
+      <c r="R4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="S4" s="0" t="n">
+      <c r="S4" s="4" t="n">
         <v>1</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="L5" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="M5" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="N5" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="O5" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="P5" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="4" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="R5" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="S5" s="4" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="H6" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="L6" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="M6" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="N6" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="O6" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="P6" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="4" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="R6" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="S6" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="L7" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="M7" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="N7" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="O7" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="P7" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="4" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="R7" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="S7" s="4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="L8" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="M8" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="N8" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="O8" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="P8" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="4" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="R8" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="S8" s="4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="L9" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="M9" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="N9" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="O9" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="P9" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="4" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="R9" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="S9" s="4" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+    </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
       <c r="K11" s="11"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G26" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="H26" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="I26" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="J26" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="K26" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="L26" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="M26" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="N26" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="O26" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="P26" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="Q26" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="R26" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="S26" s="0" t="n">
-        <v>19</v>
-      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -763,6 +1397,7 @@
     <hyperlink ref="F3" r:id="rId3" display="17@gmail.com"/>
     <hyperlink ref="J3" r:id="rId4" display="17@ufps.edu.co"/>
     <hyperlink ref="F4" r:id="rId5" display="y@gmail.com"/>
+    <hyperlink ref="J5" r:id="rId6" display="12@ufps.edu.co"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -779,40 +1414,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="A1:F4"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="A8:F9 A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.91"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -856,27 +1491,316 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="4" t="n">
         <v>1</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>9</v>
+      </c>
+    </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="11"/>
+      <c r="A8" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -894,16 +1818,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F4"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.68"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
@@ -911,22 +1835,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -948,7 +1872,7 @@
       <c r="F2" s="8" t="n">
         <v>1212</v>
       </c>
-      <c r="G2" s="15"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="n">
@@ -971,24 +1895,444 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="4" t="n">
         <v>1</v>
       </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>